<commit_message>
Retook measurements using laptop for 512B packets at 100ms
Signed-off-by:Ashish Kashinath<akashina@eng.ucsd.edu>
</commit_message>
<xml_diff>
--- a/SwitchProcessingTime/laptop_measurements_100ms.xlsx
+++ b/SwitchProcessingTime/laptop_measurements_100ms.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak7\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak7\OneDrive - UC San Diego\Illinois Urbana Champaign\Repositories\qos_synthesis\SwitchProcessingTime\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" tabRatio="360" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" tabRatio="360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="256B" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,6 +112,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -128,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,9 +159,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -170,6 +179,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,37 +522,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,8 +565,8 @@
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
       <c r="H3" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,32 +584,32 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>348.63600000000002</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>361.25099999999998</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>392.69499999999999</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>376.709</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>301.23399999999998</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>312.45100000000002</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>310.387</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>320.12900000000002</v>
       </c>
     </row>
@@ -601,32 +617,32 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>345.41</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>373.19900000000001</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>361.40600000000001</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>389.36099999999999</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>305.64100000000002</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>299.928</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>308.47500000000002</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="9">
         <v>321.63299999999998</v>
       </c>
     </row>
@@ -634,32 +650,32 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>351.60899999999998</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>388.80399999999997</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>349.62700000000001</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>405.03100000000001</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>299.38900000000001</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>308.38900000000001</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>310.15300000000002</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <v>324.68299999999999</v>
       </c>
     </row>
@@ -667,32 +683,32 @@
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>359.154</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>364.255</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>361.34</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>410.44600000000003</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>304.53800000000001</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <v>312.44200000000001</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <v>311.185</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <v>329.642</v>
       </c>
     </row>
@@ -700,32 +716,32 @@
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>349.35</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>365.78800000000001</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>369.89699999999999</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>432.34899999999999</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="9">
         <v>307.298</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <v>313.29199999999997</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <v>299.02</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <v>328.56</v>
       </c>
     </row>
@@ -733,32 +749,32 @@
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>351.53</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>379.21199999999999</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>388.154</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>370.017</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>297.98200000000003</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <v>311.63600000000002</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>305.459</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="9">
         <v>317.67</v>
       </c>
     </row>
@@ -766,32 +782,32 @@
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>357.221</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>380.88299999999998</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>384.58600000000001</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>437.08699999999999</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <v>293.553</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <v>316.815</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>314.46699999999998</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="9">
         <v>322.536</v>
       </c>
     </row>
@@ -799,32 +815,32 @@
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>393.14699999999999</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>375.76499999999999</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>373.74799999999999</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>390.60599999999999</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="9">
         <v>299.73</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="9">
         <v>312.41300000000001</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>301.83</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <v>328.83800000000002</v>
       </c>
     </row>
@@ -832,32 +848,32 @@
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>357.99</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>366.58499999999998</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>356.46800000000002</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>396.67200000000003</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="9">
         <v>298.64100000000002</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <v>312.25299999999999</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>301.93900000000002</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <v>331.678</v>
       </c>
     </row>
@@ -865,85 +881,85 @@
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>361.85899999999998</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>407.26</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>361.51900000000001</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>400.303</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="9">
         <v>293.077</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <v>329.01100000000002</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>313.41199999999998</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <v>330.01499999999999</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <f>AVERAGE(B4:B13)</f>
         <v>357.59060000000005</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <f>AVERAGE(C4:C13)</f>
         <v>376.30019999999996</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <f>AVERAGE(D4:D13)</f>
         <v>369.94399999999996</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <f>AVERAGE(E4:E13)</f>
         <v>400.85809999999998</v>
       </c>
-      <c r="F15" s="9"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="9">
         <f>AVERAGE(H4:H13)</f>
         <v>300.10830000000004</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="9">
         <f>AVERAGE(I4:I13)</f>
         <v>312.863</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
         <f>AVERAGE(J4:J13)</f>
         <v>307.6327</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="9">
         <f>AVERAGE(K4:K13)</f>
         <v>325.53840000000002</v>
       </c>
@@ -952,39 +968,39 @@
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <f>_xlfn.STDEV.P(B4:B13)</f>
         <v>12.861519896186447</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <f>_xlfn.STDEV.P(C4:C13)</f>
         <v>13.155589951043622</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <f>_xlfn.STDEV.P(D4:D13)</f>
         <v>13.749046657859589</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <f>_xlfn.STDEV.P(E4:E13)</f>
         <v>20.501277547752967</v>
       </c>
-      <c r="F16" s="9"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="9">
         <f>_xlfn.STDEV.P(H4:H13)</f>
         <v>4.5048613752256594</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="9">
         <f>_xlfn.STDEV.P(I4:I13)</f>
         <v>6.8287499881017801</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="9">
         <f>_xlfn.STDEV.P(J4:J13)</f>
         <v>5.0236189156821993</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="9">
         <f>_xlfn.STDEV.P(K4:K13)</f>
         <v>4.5908951893938905</v>
       </c>
@@ -993,39 +1009,39 @@
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <f>(B16*100)/B15</f>
         <v>3.5967164394663742</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <f t="shared" ref="C17:E17" si="0">(C16*100)/C15</f>
         <v>3.496035864728114</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <f t="shared" si="0"/>
         <v>3.7165210566625193</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <f t="shared" si="0"/>
         <v>5.1143478322511049</v>
       </c>
-      <c r="F17" s="9"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="9">
         <f>(H16*100)/H15</f>
         <v>1.5010785690451278</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <f t="shared" ref="I17:K17" si="1">(I16*100)/I15</f>
         <v>2.1826646129781344</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="9">
         <f t="shared" si="1"/>
         <v>1.6329924990685967</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="9">
         <f t="shared" si="1"/>
         <v>1.4102468984899754</v>
       </c>
@@ -1034,24 +1050,24 @@
       <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <f>(E15-B15)/3</f>
         <v>14.422499999999976</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="9">
         <f>(K15-H15)/3</f>
         <v>8.4766999999999939</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1064,9 +1080,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1085,21 +1101,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1115,7 +1131,7 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="3"/>
       <c r="H2" s="1" t="s">
         <v>0</v>
@@ -1146,14 +1162,14 @@
       <c r="E3" s="3">
         <v>397.75</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="10"/>
       <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="3">
         <v>312.745</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="17">
         <v>324.82900000000001</v>
       </c>
       <c r="J3" s="3">
@@ -1179,14 +1195,14 @@
       <c r="E4" s="3">
         <v>405.25599999999997</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="3">
         <v>309.62</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="17">
         <v>335.23700000000002</v>
       </c>
       <c r="J4" s="3">
@@ -1212,14 +1228,14 @@
       <c r="E5" s="3">
         <v>407.74099999999999</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="3">
         <v>297.34399999999999</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="17">
         <v>323.04899999999998</v>
       </c>
       <c r="J5" s="3">
@@ -1245,14 +1261,14 @@
       <c r="E6" s="3">
         <v>399.45</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="3">
         <v>296.16800000000001</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="17">
         <v>326.99400000000003</v>
       </c>
       <c r="J6" s="3">
@@ -1278,14 +1294,14 @@
       <c r="E7" s="3">
         <v>403.214</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="3">
         <v>310.54599999999999</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="17">
         <v>321.00700000000001</v>
       </c>
       <c r="J7" s="3">
@@ -1311,14 +1327,14 @@
       <c r="E8" s="3">
         <v>435.23</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="3">
         <v>313.40800000000002</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="17">
         <v>321.339</v>
       </c>
       <c r="J8" s="3">
@@ -1344,14 +1360,14 @@
       <c r="E9" s="3">
         <v>388.15300000000002</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="3">
         <v>307.38600000000002</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="17">
         <v>320.04899999999998</v>
       </c>
       <c r="J9" s="3">
@@ -1377,14 +1393,14 @@
       <c r="E10" s="3">
         <v>403.48500000000001</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="3">
         <v>306.54000000000002</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="17">
         <v>330.44600000000003</v>
       </c>
       <c r="J10" s="3">
@@ -1410,14 +1426,14 @@
       <c r="E11" s="3">
         <v>400.20699999999999</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="3">
         <v>308.33800000000002</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="17">
         <v>325.60700000000003</v>
       </c>
       <c r="J11" s="3">
@@ -1443,14 +1459,14 @@
       <c r="E12" s="3">
         <v>395.51</v>
       </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="3">
         <v>308.25200000000001</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="17">
         <v>321.93599999999998</v>
       </c>
       <c r="J12" s="3">
@@ -1476,14 +1492,14 @@
       <c r="E13" s="3">
         <v>407.976</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="3">
         <v>317.185</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="17">
         <v>326.27800000000002</v>
       </c>
       <c r="J13" s="3">
@@ -1507,14 +1523,14 @@
         <v>404.62299999999999</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="11"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="3">
         <v>307.702</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="17">
         <v>323.08100000000002</v>
       </c>
       <c r="J14" s="3">
@@ -1528,10 +1544,10 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="11"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="17"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
@@ -1555,7 +1571,7 @@
         <f>AVERAGE(E3:E14)</f>
         <v>403.9974545454545</v>
       </c>
-      <c r="F16" s="11"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="4" t="s">
         <v>5</v>
       </c>
@@ -1563,7 +1579,7 @@
         <f>AVERAGE(H3:H14)</f>
         <v>307.93616666666668</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="17">
         <f>AVERAGE(I3:I14)</f>
         <v>324.98766666666666</v>
       </c>
@@ -1596,7 +1612,7 @@
         <f t="shared" si="0"/>
         <v>11.301393320082559</v>
       </c>
-      <c r="F17" s="11"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="3" t="s">
         <v>6</v>
       </c>
@@ -1604,7 +1620,7 @@
         <f>_xlfn.STDEV.P(H3:H14)</f>
         <v>5.7843541966430649</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="17">
         <f t="shared" ref="I17:K17" si="1">_xlfn.STDEV.P(I3:I14)</f>
         <v>4.1952026040334456</v>
       </c>
@@ -1637,7 +1653,7 @@
         <f t="shared" si="2"/>
         <v>2.7973922095123047</v>
       </c>
-      <c r="F18" s="11"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1645,7 +1661,7 @@
         <f>(H17*100)/H16</f>
         <v>1.878426382732914</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="17">
         <f t="shared" ref="I18:K18" si="3">(I17*100)/I16</f>
         <v>1.2908805577340203</v>
       </c>
@@ -1669,7 +1685,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="10"/>
       <c r="G19" s="5" t="s">
         <v>8</v>
       </c>
@@ -1680,6 +1696,14 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="18">
+        <v>425486</v>
+      </c>
+      <c r="I20">
+        <v>322.94099999999997</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1713,595 +1737,595 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="11">
         <v>340.08800000000002</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>373.39600000000002</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>397.50799999999998</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>474.49299999999999</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="F3" s="13"/>
+      <c r="G3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="11">
         <v>301.43099999999998</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>326.334</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>332.464</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>371.923</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="12">
+      <c r="A4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
         <v>373.35</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>429.2</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>392.60199999999998</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>417.62799999999999</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="12">
+      <c r="F4" s="13"/>
+      <c r="G4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="11">
         <v>308.48200000000003</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <v>340.697</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <v>328.12799999999999</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <v>365.416</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="12">
+      <c r="A5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
         <v>388.16899999999998</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>389</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>395.92</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>454.637</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="12">
+      <c r="F5" s="13"/>
+      <c r="G5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="11">
         <v>310.02100000000002</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>329.82400000000001</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>339.69099999999997</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>376.58499999999998</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="12">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11">
         <v>352.89</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>415.76900000000001</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>407.65300000000002</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>432.887</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="12">
+      <c r="F6" s="13"/>
+      <c r="G6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="11">
         <v>301.82100000000003</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <v>336.01400000000001</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="11">
         <v>332.76100000000002</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="11">
         <v>369.697</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11">
         <v>374.77800000000002</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>377.78899999999999</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>417.35199999999998</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>458.10500000000002</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="12">
+      <c r="F7" s="13"/>
+      <c r="G7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="11">
         <v>304.95299999999997</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>327.42599999999999</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>333.31599999999997</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <v>366.471</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="A8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="11">
         <v>376.61799999999999</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>378.16399999999999</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>399.72800000000001</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>412.86599999999999</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="12">
+      <c r="F8" s="13"/>
+      <c r="G8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="11">
         <v>311.18299999999999</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>321.31299999999999</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="11">
         <v>332.41699999999997</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="11">
         <v>363.81799999999998</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="12">
+      <c r="A9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="11">
         <v>379.61500000000001</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>384.38900000000001</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>426.65899999999999</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>418.21600000000001</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="12">
+      <c r="F9" s="13"/>
+      <c r="G9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="11">
         <v>304.40699999999998</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="11">
         <v>318.87599999999998</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="11">
         <v>347.93299999999999</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="11">
         <v>367.69099999999997</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="12">
+      <c r="A10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="11">
         <v>376.43</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>361.86700000000002</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>407.90100000000001</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>418.28800000000001</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="12">
+      <c r="F10" s="13"/>
+      <c r="G10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="11">
         <v>303.54599999999999</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="11">
         <v>309.09199999999998</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="11">
         <v>346.81</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="11">
         <v>369.548</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="12">
+      <c r="A11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11">
         <v>369.28500000000003</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>359.80500000000001</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>445.76299999999998</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>402.62799999999999</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="12">
+      <c r="F11" s="13"/>
+      <c r="G11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="11">
         <v>308.73700000000002</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="11">
         <v>307.51799999999997</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="11">
         <v>345.24099999999999</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="11">
         <v>371.52499999999998</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="12">
+      <c r="A12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="11">
         <v>370.86099999999999</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>384.73899999999998</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>418.14299999999997</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>422.084</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="12">
+      <c r="F12" s="13"/>
+      <c r="G12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="11">
         <v>311.46899999999999</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="11">
         <v>336.43200000000002</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="11">
         <v>339.85199999999998</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="11">
         <v>370.983</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="12">
+      <c r="A13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="11">
         <v>376.38799999999998</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>405.74200000000002</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="11">
         <v>386.19</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>431.08800000000002</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="12">
+      <c r="F13" s="13"/>
+      <c r="G13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="11">
         <v>309.589</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="11">
         <v>326.99599999999998</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="11">
         <v>336.803</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="11">
         <v>376.42</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="12">
+      <c r="A14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="11">
         <v>310.06700000000001</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="11">
         <v>329.928</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="11">
         <v>332.65600000000001</v>
       </c>
-      <c r="K14" s="12"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <f>AVERAGE(B3:B13)</f>
         <v>370.77018181818175</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <f>AVERAGE(C3:C13)</f>
         <v>387.26000000000005</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <f>AVERAGE(D3:D13)</f>
         <v>408.67445454545447</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <f>AVERAGE(E3:E13)</f>
         <v>431.17454545454547</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="15" t="s">
+      <c r="F16" s="13"/>
+      <c r="G16" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="11">
         <f>AVERAGE(H3:H14)</f>
         <v>307.1421666666667</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="11">
         <f>AVERAGE(I3:I14)</f>
         <v>325.87083333333339</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="11">
         <f>AVERAGE(J3:J14)</f>
         <v>337.33933333333329</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="11">
         <f>AVERAGE(K3:K13)</f>
         <v>370.00700000000001</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <f>_xlfn.STDEV.P(B3:B13)</f>
         <v>12.666237683615886</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <f t="shared" ref="C17:E17" si="0">_xlfn.STDEV.P(C3:C13)</f>
         <v>20.657742801099143</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <f t="shared" si="0"/>
         <v>16.505861732144158</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <f t="shared" si="0"/>
         <v>21.117434866452012</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="10" t="s">
+      <c r="F17" s="13"/>
+      <c r="G17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <f>_xlfn.STDEV.P(H3:H14)</f>
         <v>3.5161061994137182</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="11">
         <f t="shared" ref="I17:K17" si="1">_xlfn.STDEV.P(I3:I14)</f>
         <v>9.8246363871081304</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="11">
         <f t="shared" si="1"/>
         <v>6.2477728076135701</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="11">
         <f t="shared" si="1"/>
         <v>3.918250351647</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <f>(B17*100)/B16</f>
         <v>3.4161964215955085</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <f t="shared" ref="C18:E18" si="2">(C17*100)/C16</f>
         <v>5.3343342460102106</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <f t="shared" si="2"/>
         <v>4.0388777787695824</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="11">
         <f t="shared" si="2"/>
         <v>4.8976534188004885</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="10" t="s">
+      <c r="F18" s="13"/>
+      <c r="G18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="11">
         <f>(H17*100)/H16</f>
         <v>1.1447813361392529</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="11">
         <f t="shared" ref="I18:K18" si="3">(I17*100)/I16</f>
         <v>3.0148866919484343</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="11">
         <f t="shared" si="3"/>
         <v>1.8520736215008737</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="11">
         <f t="shared" si="3"/>
         <v>1.0589665470239753</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="11">
         <f>(E16-B16)/3</f>
         <v>20.134787878787904</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="16" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="11">
         <f>(K16-H16)/3</f>
         <v>20.954944444444436</v>
       </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2316,7 +2340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -2336,21 +2360,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>

</xml_diff>